<commit_message>
regstaratieproces aanmaken en versturing van registratiemail
</commit_message>
<xml_diff>
--- a/LogboekFotoSjaak.xlsx
+++ b/LogboekFotoSjaak.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="totaal" sheetId="5" r:id="rId1"/>
     <sheet name="weeknr 46" sheetId="1" r:id="rId2"/>
+    <sheet name="weeknr 47" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Logboek</t>
   </si>
@@ -72,6 +73,9 @@
   </si>
   <si>
     <t>Verder gewerkt aan het inlogsysteem</t>
+  </si>
+  <si>
+    <t>script geschreven voor activatiemail</t>
   </si>
 </sst>
 </file>
@@ -480,7 +484,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,11 +542,17 @@
       </c>
       <c r="B7" s="4">
         <f>'weeknr 46'!$G$5</f>
+        <v>0.27083333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4">
+        <f>'weeknr 47'!$G$5</f>
         <v>0.13541666666666669</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -550,7 +560,7 @@
       </c>
       <c r="B9" s="14">
         <f>SUM(B7:B8)</f>
-        <v>0.13541666666666669</v>
+        <v>0.40625000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -565,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +626,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G5" s="9">
         <f>SUM(G6:G998)</f>
-        <v>0.13541666666666669</v>
+        <v>0.27083333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -685,7 +695,10 @@
       <c r="F8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9">
+        <f>D8-C8</f>
+        <v>0.13541666666666669</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
@@ -1647,4 +1660,316 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="98.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="12"/>
+      <c r="G5" s="9">
+        <f>SUM(G6:G998)</f>
+        <v>0.13541666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <f>B7</f>
+        <v>41232</v>
+      </c>
+      <c r="B7" s="8">
+        <v>41232</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="9">
+        <f>D7-C7</f>
+        <v>0.13541666666666669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <f t="shared" ref="A8:A23" si="0">B8</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
wachtwoord zijigen en registratie
</commit_message>
<xml_diff>
--- a/LogboekFotoSjaak.xlsx
+++ b/LogboekFotoSjaak.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="totaal" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Logboek</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>script geschreven voor activatiemail</t>
+  </si>
+  <si>
+    <t>activatie proces anngemaakt, wachtword word gewijzigd bij administratie</t>
   </si>
 </sst>
 </file>
@@ -483,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +554,7 @@
       </c>
       <c r="B8" s="4">
         <f>'weeknr 47'!$G$5</f>
-        <v>0.13541666666666669</v>
+        <v>0.27083333333333337</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,7 +563,7 @@
       </c>
       <c r="B9" s="14">
         <f>SUM(B7:B8)</f>
-        <v>0.40625000000000006</v>
+        <v>0.54166666666666674</v>
       </c>
     </row>
   </sheetData>
@@ -1666,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,7 +1728,7 @@
       <c r="F5" s="12"/>
       <c r="G5" s="9">
         <f>SUM(G6:G998)</f>
-        <v>0.13541666666666669</v>
+        <v>0.27083333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1777,20 +1780,30 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f t="shared" ref="A8:A23" si="0">B8</f>
-        <v>0</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="9"/>
+        <v>41235</v>
+      </c>
+      <c r="B8" s="8">
+        <v>41235</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="9">
+        <f>D8-C8</f>
+        <v>0.13541666666666669</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A9" s="15"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1799,10 +1812,7 @@
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A10" s="15"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -1811,10 +1821,7 @@
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A11" s="15"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1823,10 +1830,7 @@
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A12" s="15"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1835,10 +1839,7 @@
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A13" s="15"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1847,10 +1848,7 @@
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A14" s="15"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1859,10 +1857,7 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A15" s="15"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1871,10 +1866,7 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A16" s="15"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1883,10 +1875,7 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A17" s="15"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1895,10 +1884,7 @@
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A18" s="15"/>
       <c r="B18" s="8"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1907,10 +1893,7 @@
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A19" s="15"/>
       <c r="B19" s="8"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1919,10 +1902,7 @@
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A20" s="15"/>
       <c r="B20" s="8"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1931,10 +1911,7 @@
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A21" s="15"/>
       <c r="B21" s="8"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1943,10 +1920,7 @@
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A22" s="15"/>
       <c r="B22" s="8"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1955,10 +1929,7 @@
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A23" s="15"/>
       <c r="B23" s="8"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>

</xml_diff>